<commit_message>
Altered default excel file
</commit_message>
<xml_diff>
--- a/Slooier_voorraad/Slooier_voorraad/Voorbeeld_Data/bestellijst wijngo materialenV2.xlsx
+++ b/Slooier_voorraad/Slooier_voorraad/Voorbeeld_Data/bestellijst wijngo materialenV2.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\Red Darkness\Documents\Documenten\Github\Repositories\Slooier_management\Slooier_voorraad\Slooier_voorraad\Voorbeeld_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D5F96A4-9DC4-4127-A1B2-9C5C7A04087C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{221DAEBD-EC14-4ED2-847C-5E41862ACF72}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Artikelen" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="326">
   <si>
     <t>hang en sluitwerk</t>
   </si>
@@ -996,6 +996,9 @@
   </si>
   <si>
     <t>Prijs</t>
+  </si>
+  <si>
+    <t>Voorraad</t>
   </si>
 </sst>
 </file>
@@ -1388,11 +1391,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F310"/>
+  <dimension ref="A1:I310"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
+      <selection pane="bottomLeft" activeCell="E3" sqref="E3:E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -1401,11 +1404,12 @@
     <col min="2" max="2" width="11" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="53" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="0" style="3" hidden="1"/>
-    <col min="7" max="16384" width="9.140625" style="3" hidden="1"/>
+    <col min="5" max="5" width="9.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="0" style="3" hidden="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="3" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>321</v>
       </c>
@@ -1418,16 +1422,20 @@
       <c r="D1" s="1" t="s">
         <v>324</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="1" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>259</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
       <c r="D2" s="1"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" s="5"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4" t="s">
         <v>51</v>
@@ -1438,8 +1446,9 @@
       <c r="D3" s="2">
         <v>7.16</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" s="4"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="4" t="s">
         <v>112</v>
@@ -1447,8 +1456,9 @@
       <c r="C4" s="4" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" s="4"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="4" t="s">
         <v>76</v>
@@ -1456,38 +1466,43 @@
       <c r="C5" s="4" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" s="4"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
         <v>75</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" s="4"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" s="4"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" s="4"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
         <v>78</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9" s="4"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="4" t="s">
         <v>77</v>
@@ -1495,15 +1510,17 @@
       <c r="C10" s="4" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10" s="4"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11" s="4"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="4" t="s">
         <v>70</v>
@@ -1511,8 +1528,9 @@
       <c r="C12" s="4" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12" s="4"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="4" t="s">
         <v>68</v>
@@ -1520,8 +1538,9 @@
       <c r="C13" s="4" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13" s="4"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="4" t="s">
         <v>79</v>
@@ -1529,8 +1548,9 @@
       <c r="C14" s="4" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14" s="4"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="4" t="s">
         <v>81</v>
@@ -1538,8 +1558,9 @@
       <c r="C15" s="4" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E15" s="4"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="4" t="s">
         <v>67</v>
@@ -1547,8 +1568,9 @@
       <c r="C16" s="4" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16" s="4"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="4" t="s">
         <v>237</v>
@@ -1556,8 +1578,9 @@
       <c r="C17" s="4" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17" s="4"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="4" t="s">
         <v>66</v>
@@ -1565,8 +1588,9 @@
       <c r="C18" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18" s="4"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="4" t="s">
         <v>49</v>
@@ -1574,8 +1598,9 @@
       <c r="C19" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19" s="4"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="4" t="s">
         <v>238</v>
@@ -1583,8 +1608,9 @@
       <c r="C20" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E20" s="4"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="4" t="s">
         <v>239</v>
@@ -1592,43 +1618,48 @@
       <c r="C21" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E21" s="4"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E22" s="4"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E23" s="4"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E24" s="4"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="2" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E26" s="4"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="4" t="s">
         <v>52</v>
@@ -1636,8 +1667,9 @@
       <c r="C27" s="4" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E27" s="4"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="4" t="s">
         <v>53</v>
@@ -1645,8 +1677,9 @@
       <c r="C28" s="4" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E28" s="4"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="4">
         <v>301826</v>
@@ -1654,8 +1687,9 @@
       <c r="C29" s="4" t="s">
         <v>285</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E29" s="4"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="4">
         <v>999058</v>
@@ -1666,8 +1700,9 @@
       <c r="D30" s="2">
         <v>53.48</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E30" s="4"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" s="4">
         <v>200084</v>
@@ -1678,16 +1713,18 @@
       <c r="D31" s="2">
         <v>9.44</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E31" s="4"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>258</v>
       </c>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
       <c r="D32" s="1"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E32" s="5"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
       <c r="B33" s="2" t="s">
         <v>50</v>
@@ -1698,8 +1735,9 @@
       <c r="D33" s="2">
         <v>3.24</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E33" s="4"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="B34" s="4">
         <v>200457</v>
@@ -1710,8 +1748,9 @@
       <c r="D34" s="2">
         <v>20.59</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E34" s="4"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
       <c r="B35" s="4">
         <v>200043</v>
@@ -1722,8 +1761,9 @@
       <c r="D35" s="2">
         <v>11.24</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E35" s="4"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
       <c r="B36" s="4">
         <v>200575</v>
@@ -1734,8 +1774,9 @@
       <c r="D36" s="2">
         <v>16.32</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E36" s="4"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
       <c r="B37" s="4">
         <v>200337</v>
@@ -1746,8 +1787,9 @@
       <c r="D37" s="2">
         <v>17.600000000000001</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E37" s="4"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
       <c r="B38" s="4">
         <v>200131</v>
@@ -1758,8 +1800,9 @@
       <c r="D38" s="2">
         <v>13.99</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E38" s="4"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
       <c r="B39" s="4">
         <v>201563</v>
@@ -1767,8 +1810,9 @@
       <c r="C39" s="4" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E39" s="4"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="4"/>
       <c r="B40" s="4">
         <v>201756</v>
@@ -1776,8 +1820,9 @@
       <c r="C40" s="4" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E40" s="4"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="4"/>
       <c r="B41" s="4">
         <v>275015</v>
@@ -1788,8 +1833,9 @@
       <c r="D41" s="2">
         <v>8.8000000000000007</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E41" s="4"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="4"/>
       <c r="B42" s="4">
         <v>330750</v>
@@ -1801,7 +1847,7 @@
         <v>9.5500000000000007</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="4"/>
       <c r="B43" s="4">
         <v>330775</v>
@@ -1813,7 +1859,7 @@
         <v>25.66</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="4"/>
       <c r="B44" s="4" t="s">
         <v>187</v>
@@ -1821,8 +1867,9 @@
       <c r="C44" s="4" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E44" s="4"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="4"/>
       <c r="B45" s="4" t="s">
         <v>188</v>
@@ -1830,8 +1877,9 @@
       <c r="C45" s="4" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E45" s="4"/>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="4"/>
       <c r="B46" s="4" t="s">
         <v>189</v>
@@ -1839,16 +1887,18 @@
       <c r="C46" s="4" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E46" s="4"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B47" s="5"/>
       <c r="C47" s="5"/>
       <c r="D47" s="1"/>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E47" s="5"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="4"/>
       <c r="B48" s="4">
         <v>305466</v>
@@ -1859,8 +1909,9 @@
       <c r="D48" s="2">
         <v>31.01</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E48" s="4"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="4"/>
       <c r="B49" s="4">
         <v>305465</v>
@@ -1871,8 +1922,9 @@
       <c r="D49" s="2">
         <v>31.01</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E49" s="4"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="4"/>
       <c r="B50" s="4">
         <v>950127</v>
@@ -1883,8 +1935,9 @@
       <c r="D50" s="2">
         <v>14.76</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E50" s="4"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="4"/>
       <c r="B51" s="4">
         <v>950126</v>
@@ -1895,8 +1948,9 @@
       <c r="D51" s="2">
         <v>14.76</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E51" s="4"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="4"/>
       <c r="B52" s="4">
         <v>950177</v>
@@ -1904,8 +1958,9 @@
       <c r="C52" s="4" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E52" s="4"/>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="4"/>
       <c r="B53" s="4">
         <v>950176</v>
@@ -1913,8 +1968,9 @@
       <c r="C53" s="4" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E53" s="4"/>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="4"/>
       <c r="B54" s="4">
         <v>313139</v>
@@ -1925,8 +1981,9 @@
       <c r="D54" s="2">
         <v>3.55</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E54" s="4"/>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="4"/>
       <c r="B55" s="4">
         <v>313118</v>
@@ -1934,8 +1991,9 @@
       <c r="C55" s="4" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E55" s="4"/>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="4"/>
       <c r="B56" s="2" t="s">
         <v>220</v>
@@ -1943,8 +2001,9 @@
       <c r="C56" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E56" s="4"/>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="4"/>
       <c r="B57" s="2" t="s">
         <v>83</v>
@@ -1952,8 +2011,9 @@
       <c r="C57" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E57" s="4"/>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="4"/>
       <c r="B58" s="4" t="s">
         <v>229</v>
@@ -1961,8 +2021,9 @@
       <c r="C58" s="4" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E58" s="4"/>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="4"/>
       <c r="B59" s="2" t="s">
         <v>201</v>
@@ -1970,8 +2031,9 @@
       <c r="C59" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E59" s="4"/>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="4"/>
       <c r="B60" s="2" t="s">
         <v>240</v>
@@ -1979,8 +2041,9 @@
       <c r="C60" s="4" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E60" s="4"/>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="4"/>
       <c r="B61" s="2" t="s">
         <v>200</v>
@@ -1988,8 +2051,9 @@
       <c r="C61" s="4" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E61" s="4"/>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="4"/>
       <c r="B62" s="4">
         <v>413980</v>
@@ -1998,7 +2062,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="4"/>
       <c r="B63" s="4">
         <v>413983</v>
@@ -2007,7 +2071,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="4"/>
       <c r="B64" s="4">
         <v>255234</v>
@@ -2018,8 +2082,9 @@
       <c r="D64" s="2">
         <v>16.47</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E64" s="4"/>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="4"/>
       <c r="B65" s="4">
         <v>305101</v>
@@ -2030,8 +2095,9 @@
       <c r="D65" s="2">
         <v>36.28</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E65" s="4"/>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="4"/>
       <c r="B66" s="4">
         <v>220005</v>
@@ -2042,8 +2108,9 @@
       <c r="D66" s="2">
         <v>3.48</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E66" s="4"/>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="4"/>
       <c r="B67" s="2" t="s">
         <v>142</v>
@@ -2051,16 +2118,18 @@
       <c r="C67" s="4" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E67" s="4"/>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B68" s="5"/>
       <c r="C68" s="5"/>
       <c r="D68" s="1"/>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E68" s="5"/>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="4"/>
       <c r="B69" s="4">
         <v>155830</v>
@@ -2071,8 +2140,9 @@
       <c r="D69" s="2">
         <v>36.159999999999997</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E69" s="4"/>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="4"/>
       <c r="B70" s="4">
         <v>155822</v>
@@ -2083,8 +2153,9 @@
       <c r="D70" s="2">
         <v>62.72</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E70" s="4"/>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="4"/>
       <c r="B71" s="4">
         <v>155823</v>
@@ -2095,8 +2166,9 @@
       <c r="D71" s="2">
         <v>62.72</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E71" s="4"/>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="4"/>
       <c r="B72" s="4">
         <v>151255</v>
@@ -2108,7 +2180,7 @@
         <v>25.75</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="4"/>
       <c r="B73" s="4">
         <v>5128</v>
@@ -2116,8 +2188,9 @@
       <c r="C73" s="4" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E73" s="4"/>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="4"/>
       <c r="B74" s="4">
         <v>148020</v>
@@ -2129,14 +2202,15 @@
         <v>42.48</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="4"/>
       <c r="B75" s="4"/>
       <c r="C75" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E75" s="4"/>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="4"/>
       <c r="B76" s="4">
         <v>148415</v>
@@ -2147,8 +2221,9 @@
       <c r="D76" s="2">
         <v>42.08</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E76" s="4"/>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="4"/>
       <c r="B77" s="4">
         <v>148658</v>
@@ -2156,8 +2231,9 @@
       <c r="C77" s="4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E77" s="4"/>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="4"/>
       <c r="B78" s="4">
         <v>424531</v>
@@ -2165,8 +2241,9 @@
       <c r="C78" s="4" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E78" s="4"/>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="4"/>
       <c r="B79" s="4">
         <v>424510</v>
@@ -2174,8 +2251,9 @@
       <c r="C79" s="4" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E79" s="4"/>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="4"/>
       <c r="B80" s="4">
         <v>424515</v>
@@ -2183,15 +2261,17 @@
       <c r="C80" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E80" s="4"/>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="4"/>
       <c r="B81" s="4"/>
       <c r="C81" s="4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E81" s="4"/>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="4"/>
       <c r="B82" s="4">
         <v>155545</v>
@@ -2203,14 +2283,15 @@
         <v>182.04</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="4"/>
       <c r="B83" s="4"/>
       <c r="C83" s="4" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E83" s="4"/>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="4"/>
       <c r="B84" s="4">
         <v>970420</v>
@@ -2218,8 +2299,9 @@
       <c r="C84" s="4" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E84" s="4"/>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="4"/>
       <c r="B85" s="4">
         <v>148735</v>
@@ -2230,8 +2312,9 @@
       <c r="D85" s="2">
         <v>7.81</v>
       </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E85" s="4"/>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="4"/>
       <c r="B86" s="4">
         <v>150922</v>
@@ -2243,7 +2326,7 @@
         <v>140.97</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="4"/>
       <c r="B87" s="4">
         <v>150935</v>
@@ -2254,8 +2337,9 @@
       <c r="D87" s="2">
         <v>59.81</v>
       </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E87" s="4"/>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="4"/>
       <c r="B88" s="4">
         <v>151296</v>
@@ -2266,8 +2350,9 @@
       <c r="D88" s="2">
         <v>6.9</v>
       </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E88" s="4"/>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="4"/>
       <c r="B89" s="4">
         <v>525086</v>
@@ -2275,8 +2360,9 @@
       <c r="C89" s="4" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E89" s="4"/>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="4"/>
       <c r="B90" s="4">
         <v>429659</v>
@@ -2284,8 +2370,9 @@
       <c r="C90" s="4" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E90" s="4"/>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="4"/>
       <c r="B91" s="4">
         <v>155628</v>
@@ -2297,7 +2384,7 @@
         <v>170.93</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="4"/>
       <c r="B92" s="4">
         <v>424575</v>
@@ -2305,8 +2392,9 @@
       <c r="C92" s="4" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E92" s="4"/>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="4"/>
       <c r="B93" s="4">
         <v>525501</v>
@@ -2314,8 +2402,9 @@
       <c r="C93" s="4" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E93" s="4"/>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="4"/>
       <c r="B94" s="4">
         <v>525502</v>
@@ -2323,8 +2412,9 @@
       <c r="C94" s="4" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E94" s="4"/>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="4"/>
       <c r="B95" s="4">
         <v>525503</v>
@@ -2332,8 +2422,9 @@
       <c r="C95" s="4" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E95" s="4"/>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="4"/>
       <c r="B96" s="4">
         <v>525504</v>
@@ -2341,8 +2432,9 @@
       <c r="C96" s="4" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E96" s="4"/>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="4"/>
       <c r="B97" s="4">
         <v>525505</v>
@@ -2350,16 +2442,18 @@
       <c r="C97" s="4" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E97" s="4"/>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="4" t="s">
         <v>275</v>
       </c>
       <c r="B98" s="5"/>
       <c r="C98" s="5"/>
       <c r="D98" s="1"/>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E98" s="5"/>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="4"/>
       <c r="B99" s="2" t="s">
         <v>118</v>
@@ -2367,8 +2461,9 @@
       <c r="C99" s="4" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E99" s="4"/>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="4"/>
       <c r="B100" s="4" t="s">
         <v>119</v>
@@ -2376,8 +2471,9 @@
       <c r="C100" s="4" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E100" s="4"/>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="4"/>
       <c r="B101" s="4" t="s">
         <v>168</v>
@@ -2385,8 +2481,9 @@
       <c r="C101" s="4" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E101" s="4"/>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="4"/>
       <c r="B102" s="4" t="s">
         <v>166</v>
@@ -2394,15 +2491,17 @@
       <c r="C102" s="4" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E102" s="4"/>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="4"/>
       <c r="B103" s="4"/>
       <c r="C103" s="4" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E103" s="4"/>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="4"/>
       <c r="B104" s="4" t="s">
         <v>122</v>
@@ -2410,8 +2509,9 @@
       <c r="C104" s="4" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E104" s="4"/>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="4"/>
       <c r="B105" s="4">
         <v>524952</v>
@@ -2419,8 +2519,9 @@
       <c r="C105" s="4" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E105" s="4"/>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="4"/>
       <c r="B106" s="4">
         <v>483253</v>
@@ -2431,8 +2532,9 @@
       <c r="D106" s="2">
         <v>33.28</v>
       </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E106" s="4"/>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="4"/>
       <c r="B107" s="4">
         <v>483251</v>
@@ -2443,8 +2545,9 @@
       <c r="D107" s="2">
         <v>14.58</v>
       </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E107" s="4"/>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="4"/>
       <c r="B108" s="2" t="s">
         <v>219</v>
@@ -2452,8 +2555,9 @@
       <c r="C108" s="4" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E108" s="4"/>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="4"/>
       <c r="B109" s="4">
         <v>515182</v>
@@ -2464,8 +2568,9 @@
       <c r="D109" s="2">
         <v>17.27</v>
       </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E109" s="4"/>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="4"/>
       <c r="B110" s="4">
         <v>515184</v>
@@ -2476,8 +2581,9 @@
       <c r="D110" s="2">
         <v>34.58</v>
       </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E110" s="4"/>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="4"/>
       <c r="B111" s="4">
         <v>515185</v>
@@ -2488,16 +2594,18 @@
       <c r="D111" s="2">
         <v>57.6</v>
       </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E111" s="4"/>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="4" t="s">
         <v>26</v>
       </c>
       <c r="B112" s="5"/>
       <c r="C112" s="5"/>
       <c r="D112" s="1"/>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E112" s="5"/>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="4"/>
       <c r="B113" s="4">
         <v>516214</v>
@@ -2509,7 +2617,7 @@
         <v>7.67</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" s="4"/>
       <c r="B114" s="4">
         <v>516222</v>
@@ -2520,8 +2628,9 @@
       <c r="D114" s="2">
         <v>28.9</v>
       </c>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E114" s="4"/>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="4"/>
       <c r="B115" s="4">
         <v>516231</v>
@@ -2532,8 +2641,9 @@
       <c r="D115" s="2">
         <v>8.0500000000000007</v>
       </c>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E115" s="4"/>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="4"/>
       <c r="B116" s="4">
         <v>516301</v>
@@ -2544,8 +2654,9 @@
       <c r="D116" s="2">
         <v>7.33</v>
       </c>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E116" s="4"/>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" s="4"/>
       <c r="B117" s="4">
         <v>516302</v>
@@ -2556,8 +2667,9 @@
       <c r="D117" s="2">
         <v>7.33</v>
       </c>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E117" s="4"/>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" s="4"/>
       <c r="B118" s="4">
         <v>516305</v>
@@ -2568,8 +2680,9 @@
       <c r="D118" s="2">
         <v>7.33</v>
       </c>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E118" s="4"/>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" s="4"/>
       <c r="B119" s="4">
         <v>516287</v>
@@ -2577,8 +2690,9 @@
       <c r="C119" s="4" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E119" s="4"/>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" s="4"/>
       <c r="B120" s="4">
         <v>516254</v>
@@ -2589,8 +2703,9 @@
       <c r="D120" s="2">
         <v>6.89</v>
       </c>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E120" s="4"/>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="4"/>
       <c r="B121" s="4">
         <v>516252</v>
@@ -2601,8 +2716,9 @@
       <c r="D121" s="2">
         <v>6.89</v>
       </c>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E121" s="4"/>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" s="4"/>
       <c r="B122" s="4">
         <v>516251</v>
@@ -2613,8 +2729,9 @@
       <c r="D122" s="2">
         <v>6.89</v>
       </c>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E122" s="4"/>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" s="4"/>
       <c r="B123" s="4">
         <v>516253</v>
@@ -2625,8 +2742,9 @@
       <c r="D123" s="2">
         <v>6.89</v>
       </c>
-    </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E123" s="4"/>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" s="4"/>
       <c r="B124" s="4">
         <v>516256</v>
@@ -2634,8 +2752,9 @@
       <c r="C124" s="4" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E124" s="4"/>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" s="4"/>
       <c r="B125" s="4">
         <v>516276</v>
@@ -2646,8 +2765,9 @@
       <c r="D125" s="2">
         <v>5.88</v>
       </c>
-    </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E125" s="4"/>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" s="4"/>
       <c r="B126" s="4">
         <v>516405</v>
@@ -2658,8 +2778,9 @@
       <c r="D126" s="2">
         <v>7.34</v>
       </c>
-    </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E126" s="4"/>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" s="4"/>
       <c r="B127" s="4">
         <v>516410</v>
@@ -2670,8 +2791,9 @@
       <c r="D127" s="2">
         <v>9.8699999999999992</v>
       </c>
-    </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E127" s="4"/>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" s="4"/>
       <c r="B128" s="4">
         <v>500347</v>
@@ -2679,8 +2801,9 @@
       <c r="C128" s="4" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E128" s="4"/>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" s="4"/>
       <c r="B129" s="4" t="s">
         <v>192</v>
@@ -2688,16 +2811,18 @@
       <c r="C129" s="4" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E129" s="4"/>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" s="4" t="s">
         <v>276</v>
       </c>
       <c r="B130" s="5"/>
       <c r="C130" s="5"/>
       <c r="D130" s="1"/>
-    </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E130" s="5"/>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" s="4"/>
       <c r="B131" s="4" t="s">
         <v>65</v>
@@ -2705,8 +2830,9 @@
       <c r="C131" s="4" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E131" s="4"/>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" s="4"/>
       <c r="B132" s="4" t="s">
         <v>143</v>
@@ -2714,8 +2840,9 @@
       <c r="C132" s="4" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E132" s="4"/>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" s="4"/>
       <c r="B133" s="4" t="s">
         <v>98</v>
@@ -2723,8 +2850,9 @@
       <c r="C133" s="4" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E133" s="4"/>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" s="4"/>
       <c r="B134" s="4">
         <v>479074</v>
@@ -2732,8 +2860,9 @@
       <c r="C134" s="4" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E134" s="4"/>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" s="4"/>
       <c r="B135" s="4">
         <v>479072</v>
@@ -2741,8 +2870,9 @@
       <c r="C135" s="4" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E135" s="4"/>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" s="4"/>
       <c r="B136" s="2" t="s">
         <v>94</v>
@@ -2750,8 +2880,9 @@
       <c r="C136" s="4" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E136" s="4"/>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" s="4"/>
       <c r="B137" s="4" t="s">
         <v>93</v>
@@ -2759,8 +2890,9 @@
       <c r="C137" s="4" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E137" s="4"/>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" s="4"/>
       <c r="B138" s="4" t="s">
         <v>95</v>
@@ -2768,8 +2900,9 @@
       <c r="C138" s="4" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E138" s="4"/>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" s="4"/>
       <c r="B139" s="4" t="s">
         <v>96</v>
@@ -2777,16 +2910,18 @@
       <c r="C139" s="4" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E139" s="4"/>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" s="4" t="s">
         <v>266</v>
       </c>
       <c r="B140" s="5"/>
       <c r="C140" s="5"/>
       <c r="D140" s="1"/>
-    </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E140" s="5"/>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" s="4"/>
       <c r="B141" s="4">
         <v>516631</v>
@@ -2794,8 +2929,9 @@
       <c r="C141" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E141" s="4"/>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" s="4"/>
       <c r="B142" s="4">
         <v>516622</v>
@@ -2806,8 +2942,9 @@
       <c r="D142" s="2">
         <v>8.0500000000000007</v>
       </c>
-    </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E142" s="4"/>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" s="4"/>
       <c r="B143" s="4">
         <v>479001</v>
@@ -2818,15 +2955,17 @@
       <c r="D143" s="2">
         <v>2.1</v>
       </c>
-    </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E143" s="4"/>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" s="4"/>
       <c r="B144" s="4"/>
       <c r="C144" s="4" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E144" s="4"/>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" s="4"/>
       <c r="B145" s="4">
         <v>641383</v>
@@ -2838,7 +2977,7 @@
         <v>12.41</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" s="4"/>
       <c r="B146" s="4">
         <v>641361</v>
@@ -2849,8 +2988,9 @@
       <c r="D146" s="2">
         <v>1.25</v>
       </c>
-    </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E146" s="4"/>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" s="4"/>
       <c r="B147" s="4">
         <v>516820</v>
@@ -2858,8 +2998,9 @@
       <c r="C147" s="4" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E147" s="4"/>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" s="4"/>
       <c r="B148" s="4">
         <v>516805</v>
@@ -2867,8 +3008,9 @@
       <c r="C148" s="4" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E148" s="4"/>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" s="4"/>
       <c r="B149" s="4">
         <v>636384</v>
@@ -2880,7 +3022,7 @@
         <v>255.6</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" s="4"/>
       <c r="B150" s="4">
         <v>970104</v>
@@ -2891,8 +3033,9 @@
       <c r="D150" s="2">
         <v>26.36</v>
       </c>
-    </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E150" s="4"/>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" s="4"/>
       <c r="B151" s="4">
         <v>601429</v>
@@ -2900,8 +3043,9 @@
       <c r="C151" s="4" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E151" s="4"/>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152" s="4"/>
       <c r="B152" s="4">
         <v>507879</v>
@@ -2912,8 +3056,9 @@
       <c r="D152" s="2">
         <v>35.53</v>
       </c>
-    </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E152" s="4"/>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" s="4"/>
       <c r="B153" s="4">
         <v>507881</v>
@@ -2924,8 +3069,9 @@
       <c r="D153" s="2">
         <v>12.9</v>
       </c>
-    </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E153" s="4"/>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" s="4"/>
       <c r="B154" s="4">
         <v>507880</v>
@@ -2936,16 +3082,18 @@
       <c r="D154" s="2">
         <v>11.28</v>
       </c>
-    </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E154" s="4"/>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" s="4" t="s">
         <v>260</v>
       </c>
       <c r="B155" s="5"/>
       <c r="C155" s="5"/>
       <c r="D155" s="1"/>
-    </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E155" s="5"/>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" s="4"/>
       <c r="B156" s="4">
         <v>946015</v>
@@ -2953,8 +3101,9 @@
       <c r="C156" s="4" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E156" s="4"/>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" s="4"/>
       <c r="B157" s="4">
         <v>946296</v>
@@ -2962,8 +3111,9 @@
       <c r="C157" s="4" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E157" s="4"/>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" s="4"/>
       <c r="B158" s="4">
         <v>946012</v>
@@ -2971,8 +3121,9 @@
       <c r="C158" s="4" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E158" s="4"/>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" s="4"/>
       <c r="B159" s="4">
         <v>946294</v>
@@ -2980,8 +3131,9 @@
       <c r="C159" s="4" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E159" s="4"/>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" s="4"/>
       <c r="B160" s="4">
         <v>474409</v>
@@ -2993,7 +3145,7 @@
         <v>1.36</v>
       </c>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161" s="4"/>
       <c r="B161" s="4">
         <v>455109</v>
@@ -3001,8 +3153,9 @@
       <c r="C161" s="4" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E161" s="4"/>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162" s="4"/>
       <c r="B162" s="4">
         <v>468034</v>
@@ -3013,16 +3166,18 @@
       <c r="D162" s="2">
         <v>35.799999999999997</v>
       </c>
-    </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E162" s="4"/>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" s="4" t="s">
         <v>39</v>
       </c>
       <c r="B163" s="5"/>
       <c r="C163" s="5"/>
       <c r="D163" s="1"/>
-    </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E163" s="5"/>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164" s="4"/>
       <c r="B164" s="4">
         <v>516121</v>
@@ -3030,8 +3185,9 @@
       <c r="C164" s="4" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E164" s="4"/>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165" s="4"/>
       <c r="B165" s="4">
         <v>975264</v>
@@ -3039,8 +3195,9 @@
       <c r="C165" s="4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E165" s="4"/>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166" s="4"/>
       <c r="B166" s="4">
         <v>975014</v>
@@ -3048,8 +3205,9 @@
       <c r="C166" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E166" s="4"/>
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167" s="4"/>
       <c r="B167" s="4">
         <v>975019</v>
@@ -3057,8 +3215,9 @@
       <c r="C167" s="4" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E167" s="4"/>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" s="4"/>
       <c r="B168" s="4">
         <v>975186</v>
@@ -3066,8 +3225,9 @@
       <c r="C168" s="4" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E168" s="4"/>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" s="4"/>
       <c r="B169" s="4">
         <v>522293</v>
@@ -3075,16 +3235,18 @@
       <c r="C169" s="4" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E169" s="4"/>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170" s="4" t="s">
         <v>267</v>
       </c>
       <c r="B170" s="5"/>
       <c r="C170" s="5"/>
       <c r="D170" s="1"/>
-    </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E170" s="5"/>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171" s="4"/>
       <c r="B171" s="4">
         <v>847051</v>
@@ -3092,8 +3254,9 @@
       <c r="C171" s="4" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E171" s="4"/>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A172" s="4"/>
       <c r="B172" s="4">
         <v>515534</v>
@@ -3104,8 +3267,9 @@
       <c r="D172" s="2">
         <v>17.55</v>
       </c>
-    </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E172" s="4"/>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A173" s="4"/>
       <c r="B173" s="4">
         <v>643442</v>
@@ -3116,8 +3280,9 @@
       <c r="D173" s="2">
         <v>25.23</v>
       </c>
-    </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E173" s="4"/>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A174" s="4"/>
       <c r="B174" s="4">
         <v>515521</v>
@@ -3125,8 +3290,9 @@
       <c r="C174" s="4" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E174" s="4"/>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A175" s="4"/>
       <c r="B175" s="4">
         <v>526401</v>
@@ -3137,8 +3303,9 @@
       <c r="D175" s="2">
         <v>10.92</v>
       </c>
-    </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E175" s="4"/>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A176" s="4"/>
       <c r="B176" s="4">
         <v>526449</v>
@@ -3146,8 +3313,9 @@
       <c r="C176" s="4" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E176" s="4"/>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A177" s="4"/>
       <c r="B177" s="4">
         <v>526450</v>
@@ -3155,8 +3323,9 @@
       <c r="C177" s="4" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E177" s="4"/>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A178" s="4"/>
       <c r="B178" s="4">
         <v>526724</v>
@@ -3164,8 +3333,9 @@
       <c r="C178" s="4" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E178" s="4"/>
+    </row>
+    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179" s="4"/>
       <c r="B179" s="4">
         <v>526709</v>
@@ -3173,8 +3343,9 @@
       <c r="C179" s="4" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E179" s="4"/>
+    </row>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A180" s="4"/>
       <c r="B180" s="4">
         <v>957872</v>
@@ -3182,8 +3353,9 @@
       <c r="C180" s="4" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E180" s="4"/>
+    </row>
+    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A181" s="4"/>
       <c r="B181" s="4">
         <v>716503</v>
@@ -3191,16 +3363,18 @@
       <c r="C181" s="4" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E181" s="4"/>
+    </row>
+    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A182" s="4" t="s">
         <v>262</v>
       </c>
       <c r="B182" s="5"/>
       <c r="C182" s="5"/>
       <c r="D182" s="1"/>
-    </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E182" s="5"/>
+    </row>
+    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A183" s="4"/>
       <c r="B183" s="4">
         <v>601345</v>
@@ -3211,8 +3385,9 @@
       <c r="D183" s="2">
         <v>17.440000000000001</v>
       </c>
-    </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E183" s="4"/>
+    </row>
+    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A184" s="4"/>
       <c r="B184" s="4">
         <v>606033</v>
@@ -3220,8 +3395,9 @@
       <c r="C184" s="4" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E184" s="4"/>
+    </row>
+    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A185" s="4"/>
       <c r="B185" s="4">
         <v>623015</v>
@@ -3229,8 +3405,9 @@
       <c r="C185" s="4" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E185" s="4"/>
+    </row>
+    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A186" s="4"/>
       <c r="B186" s="4">
         <v>623119</v>
@@ -3238,8 +3415,9 @@
       <c r="C186" s="4" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E186" s="4"/>
+    </row>
+    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A187" s="4"/>
       <c r="B187" s="4">
         <v>721300</v>
@@ -3250,8 +3428,9 @@
       <c r="D187" s="2">
         <v>72.5</v>
       </c>
-    </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E187" s="4"/>
+    </row>
+    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A188" s="4"/>
       <c r="B188" s="4">
         <v>651334</v>
@@ -3262,8 +3441,9 @@
       <c r="D188" s="2">
         <v>67.75</v>
       </c>
-    </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E188" s="4"/>
+    </row>
+    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A189" s="4"/>
       <c r="B189" s="4">
         <v>514687</v>
@@ -3271,8 +3451,9 @@
       <c r="C189" s="4" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E189" s="4"/>
+    </row>
+    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A190" s="4"/>
       <c r="B190" s="4">
         <v>653022</v>
@@ -3283,8 +3464,9 @@
       <c r="D190" s="2">
         <v>4.95</v>
       </c>
-    </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E190" s="4"/>
+    </row>
+    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A191" s="4"/>
       <c r="B191" s="4">
         <v>600199</v>
@@ -3292,8 +3474,9 @@
       <c r="C191" s="4" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E191" s="4"/>
+    </row>
+    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A192" s="4"/>
       <c r="B192" s="4">
         <v>600221</v>
@@ -3301,8 +3484,9 @@
       <c r="C192" s="4" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E192" s="4"/>
+    </row>
+    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A193" s="4"/>
       <c r="B193" s="4">
         <v>487083</v>
@@ -3314,7 +3498,7 @@
         <v>1.1499999999999999</v>
       </c>
     </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A194" s="4"/>
       <c r="B194" s="4">
         <v>652621</v>
@@ -3326,7 +3510,7 @@
         <v>6.88</v>
       </c>
     </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A195" s="4"/>
       <c r="B195" s="4">
         <v>653003</v>
@@ -3338,7 +3522,7 @@
         <v>1.29</v>
       </c>
     </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A196" s="4"/>
       <c r="B196" s="4">
         <v>516662</v>
@@ -3346,8 +3530,9 @@
       <c r="C196" s="4" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E196" s="4"/>
+    </row>
+    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A197" s="4"/>
       <c r="B197" s="4">
         <v>516642</v>
@@ -3356,7 +3541,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A198" s="4"/>
       <c r="B198" s="4">
         <v>756192</v>
@@ -3364,8 +3549,9 @@
       <c r="C198" s="4" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E198" s="4"/>
+    </row>
+    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A199" s="4"/>
       <c r="B199" s="4">
         <v>830330</v>
@@ -3373,8 +3559,9 @@
       <c r="C199" s="4" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E199" s="4"/>
+    </row>
+    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A200" s="4"/>
       <c r="B200" s="4">
         <v>830331</v>
@@ -3382,8 +3569,9 @@
       <c r="C200" s="4" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E200" s="4"/>
+    </row>
+    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A201" s="4"/>
       <c r="B201" s="4" t="s">
         <v>159</v>
@@ -3391,8 +3579,9 @@
       <c r="C201" s="4" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E201" s="4"/>
+    </row>
+    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A202" s="4"/>
       <c r="B202" s="4">
         <v>521911</v>
@@ -3400,8 +3589,9 @@
       <c r="C202" s="4" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E202" s="4"/>
+    </row>
+    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A203" s="4"/>
       <c r="B203" s="4">
         <v>515590</v>
@@ -3409,8 +3599,9 @@
       <c r="C203" s="4" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E203" s="4"/>
+    </row>
+    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A204" s="4"/>
       <c r="B204" s="4">
         <v>519804</v>
@@ -3418,8 +3609,9 @@
       <c r="C204" s="4" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E204" s="4"/>
+    </row>
+    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A205" s="4"/>
       <c r="B205" s="4">
         <v>227016</v>
@@ -3427,8 +3619,9 @@
       <c r="C205" s="4" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E205" s="4"/>
+    </row>
+    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A206" s="4"/>
       <c r="B206" s="4">
         <v>646244</v>
@@ -3436,8 +3629,9 @@
       <c r="C206" s="4" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="207" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E206" s="4"/>
+    </row>
+    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A207" s="4"/>
       <c r="B207" s="4">
         <v>838209</v>
@@ -3445,16 +3639,18 @@
       <c r="C207" s="4" t="s">
         <v>293</v>
       </c>
-    </row>
-    <row r="208" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E207" s="4"/>
+    </row>
+    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A208" s="4" t="s">
         <v>261</v>
       </c>
       <c r="B208" s="5"/>
       <c r="C208" s="5"/>
       <c r="D208" s="1"/>
-    </row>
-    <row r="209" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E208" s="5"/>
+    </row>
+    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A209" s="4"/>
       <c r="B209" s="4">
         <v>711255</v>
@@ -3462,15 +3658,17 @@
       <c r="C209" s="4" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E209" s="4"/>
+    </row>
+    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A210" s="4"/>
       <c r="B210" s="4"/>
       <c r="C210" s="4" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E210" s="4"/>
+    </row>
+    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A211" s="4"/>
       <c r="B211" s="4">
         <v>711371</v>
@@ -3478,8 +3676,9 @@
       <c r="C211" s="4" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E211" s="4"/>
+    </row>
+    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A212" s="4"/>
       <c r="B212" s="4">
         <v>957700</v>
@@ -3487,8 +3686,9 @@
       <c r="C212" s="4" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E212" s="4"/>
+    </row>
+    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A213" s="4"/>
       <c r="B213" s="4">
         <v>710109</v>
@@ -3496,15 +3696,17 @@
       <c r="C213" s="4" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="214" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E213" s="4"/>
+    </row>
+    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A214" s="4"/>
       <c r="B214" s="4"/>
       <c r="C214" s="4" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="215" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E214" s="4"/>
+    </row>
+    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A215" s="4"/>
       <c r="B215" s="4">
         <v>950530</v>
@@ -3512,8 +3714,9 @@
       <c r="C215" s="4" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="216" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E215" s="4"/>
+    </row>
+    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A216" s="4"/>
       <c r="B216" s="4">
         <v>815110</v>
@@ -3521,8 +3724,9 @@
       <c r="C216" s="4" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="217" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E216" s="4"/>
+    </row>
+    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A217" s="4"/>
       <c r="B217" s="4">
         <v>815111</v>
@@ -3530,8 +3734,9 @@
       <c r="C217" s="4" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="218" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E217" s="4"/>
+    </row>
+    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A218" s="4"/>
       <c r="B218" s="4">
         <v>616865</v>
@@ -3539,8 +3744,9 @@
       <c r="C218" s="4" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="219" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E218" s="4"/>
+    </row>
+    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A219" s="4"/>
       <c r="B219" s="4">
         <v>609525</v>
@@ -3551,8 +3757,9 @@
       <c r="D219" s="2">
         <v>14.53</v>
       </c>
-    </row>
-    <row r="220" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E219" s="4"/>
+    </row>
+    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A220" s="4"/>
       <c r="B220" s="4">
         <v>990657</v>
@@ -3560,8 +3767,9 @@
       <c r="C220" s="4" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="221" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E220" s="4"/>
+    </row>
+    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A221" s="4"/>
       <c r="B221" s="2" t="s">
         <v>87</v>
@@ -3569,8 +3777,9 @@
       <c r="C221" s="4" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="222" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E221" s="4"/>
+    </row>
+    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A222" s="4"/>
       <c r="B222" s="4">
         <v>227121</v>
@@ -3578,8 +3787,9 @@
       <c r="C222" s="4" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="223" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E222" s="4"/>
+    </row>
+    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A223" s="4"/>
       <c r="B223" s="4">
         <v>226057</v>
@@ -3587,16 +3797,18 @@
       <c r="C223" s="4" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="224" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E223" s="4"/>
+    </row>
+    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A224" s="4" t="s">
         <v>278</v>
       </c>
       <c r="B224" s="5"/>
       <c r="C224" s="5"/>
       <c r="D224" s="1"/>
-    </row>
-    <row r="225" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E224" s="5"/>
+    </row>
+    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A225" s="4"/>
       <c r="B225" s="2" t="s">
         <v>145</v>
@@ -3604,15 +3816,17 @@
       <c r="C225" s="4" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="226" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E225" s="4"/>
+    </row>
+    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A226" s="4"/>
       <c r="B226" s="4"/>
       <c r="C226" s="4" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="227" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E226" s="4"/>
+    </row>
+    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A227" s="4"/>
       <c r="B227" s="4">
         <v>632178</v>
@@ -3620,8 +3834,9 @@
       <c r="C227" s="4" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="228" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E227" s="4"/>
+    </row>
+    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A228" s="4"/>
       <c r="B228" s="2" t="s">
         <v>140</v>
@@ -3629,8 +3844,9 @@
       <c r="C228" s="4" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="229" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E228" s="4"/>
+    </row>
+    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A229" s="4"/>
       <c r="B229" s="4" t="s">
         <v>60</v>
@@ -3638,8 +3854,9 @@
       <c r="C229" s="4" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="230" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E229" s="4"/>
+    </row>
+    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A230" s="4"/>
       <c r="B230" s="4">
         <v>999503</v>
@@ -3647,8 +3864,9 @@
       <c r="C230" s="4" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="231" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E230" s="4"/>
+    </row>
+    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A231" s="4"/>
       <c r="B231" s="4">
         <v>716154</v>
@@ -3656,8 +3874,9 @@
       <c r="C231" s="4" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="232" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E231" s="4"/>
+    </row>
+    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A232" s="4"/>
       <c r="B232" s="4" t="s">
         <v>151</v>
@@ -3665,8 +3884,9 @@
       <c r="C232" s="4" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="233" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E232" s="4"/>
+    </row>
+    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A233" s="4"/>
       <c r="B233" s="4">
         <v>612607</v>
@@ -3677,8 +3897,9 @@
       <c r="D233" s="2">
         <v>24.9</v>
       </c>
-    </row>
-    <row r="234" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E233" s="4"/>
+    </row>
+    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A234" s="4"/>
       <c r="B234" s="4">
         <v>612518</v>
@@ -3689,8 +3910,9 @@
       <c r="D234" s="2">
         <v>20.25</v>
       </c>
-    </row>
-    <row r="235" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E234" s="4"/>
+    </row>
+    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A235" s="4"/>
       <c r="B235" s="4">
         <v>612532</v>
@@ -3701,16 +3923,18 @@
       <c r="D235" s="2">
         <v>9.5500000000000007</v>
       </c>
-    </row>
-    <row r="236" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E235" s="4"/>
+    </row>
+    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A236" s="4" t="s">
         <v>272</v>
       </c>
       <c r="B236" s="5"/>
       <c r="C236" s="5"/>
       <c r="D236" s="1"/>
-    </row>
-    <row r="237" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E236" s="5"/>
+    </row>
+    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A237" s="4"/>
       <c r="B237" s="4" t="s">
         <v>279</v>
@@ -3722,7 +3946,7 @@
         <v>3.72</v>
       </c>
     </row>
-    <row r="238" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A238" s="4"/>
       <c r="B238" s="4" t="s">
         <v>280</v>
@@ -3734,7 +3958,7 @@
         <v>4.9400000000000004</v>
       </c>
     </row>
-    <row r="239" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A239" s="4"/>
       <c r="B239" s="4" t="s">
         <v>281</v>
@@ -3746,7 +3970,7 @@
         <v>5.68</v>
       </c>
     </row>
-    <row r="240" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A240" s="4"/>
       <c r="B240" s="4">
         <v>33253</v>
@@ -3754,8 +3978,9 @@
       <c r="C240" s="4" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="241" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E240" s="4"/>
+    </row>
+    <row r="241" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A241" s="4"/>
       <c r="B241" s="4">
         <v>33371</v>
@@ -3767,14 +3992,14 @@
         <v>24.78</v>
       </c>
     </row>
-    <row r="242" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A242" s="4"/>
       <c r="B242" s="4"/>
       <c r="C242" s="2" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="243" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A243" s="4"/>
       <c r="B243" s="4" t="s">
         <v>135</v>
@@ -3786,7 +4011,7 @@
         <v>22.9</v>
       </c>
     </row>
-    <row r="244" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A244" s="4"/>
       <c r="B244" s="4" t="s">
         <v>136</v>
@@ -3798,7 +4023,7 @@
         <v>27.12</v>
       </c>
     </row>
-    <row r="245" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A245" s="4"/>
       <c r="B245" s="4" t="s">
         <v>193</v>
@@ -3810,7 +4035,7 @@
         <v>34.159999999999997</v>
       </c>
     </row>
-    <row r="246" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A246" s="4"/>
       <c r="B246" s="4">
         <v>33503</v>
@@ -3821,8 +4046,9 @@
       <c r="D246" s="2">
         <v>7.7</v>
       </c>
-    </row>
-    <row r="247" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E246" s="4"/>
+    </row>
+    <row r="247" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A247" s="4"/>
       <c r="B247" s="4">
         <v>33190</v>
@@ -3830,16 +4056,18 @@
       <c r="C247" s="4" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="248" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E247" s="4"/>
+    </row>
+    <row r="248" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A248" s="4" t="s">
         <v>27</v>
       </c>
       <c r="B248" s="5"/>
       <c r="C248" s="5"/>
       <c r="D248" s="1"/>
-    </row>
-    <row r="249" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E248" s="5"/>
+    </row>
+    <row r="249" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A249" s="4"/>
       <c r="B249" s="4">
         <v>515502</v>
@@ -3851,7 +4079,7 @@
         <v>42.15</v>
       </c>
     </row>
-    <row r="250" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A250" s="4"/>
       <c r="B250" s="4">
         <v>515314</v>
@@ -3862,15 +4090,17 @@
       <c r="D250" s="2">
         <v>33.25</v>
       </c>
-    </row>
-    <row r="251" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E250" s="4"/>
+    </row>
+    <row r="251" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A251" s="4"/>
       <c r="B251" s="4"/>
       <c r="C251" s="4" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="252" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E251" s="4"/>
+    </row>
+    <row r="252" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A252" s="4"/>
       <c r="B252" s="4">
         <v>22023</v>
@@ -3882,15 +4112,16 @@
         <v>10.6</v>
       </c>
     </row>
-    <row r="253" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A253" s="4" t="s">
         <v>273</v>
       </c>
       <c r="B253" s="5"/>
       <c r="C253" s="5"/>
       <c r="D253" s="1"/>
-    </row>
-    <row r="254" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E253" s="5"/>
+    </row>
+    <row r="254" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A254" s="4"/>
       <c r="B254" s="4">
         <v>138903</v>
@@ -3898,22 +4129,25 @@
       <c r="C254" s="4" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="255" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E254" s="4"/>
+    </row>
+    <row r="255" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A255" s="4"/>
       <c r="B255" s="4"/>
       <c r="C255" s="4" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="256" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E255" s="4"/>
+    </row>
+    <row r="256" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A256" s="4"/>
       <c r="B256" s="4"/>
       <c r="C256" s="4" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="257" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E256" s="4"/>
+    </row>
+    <row r="257" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A257" s="4"/>
       <c r="B257" s="4">
         <v>137505</v>
@@ -3921,8 +4155,9 @@
       <c r="C257" s="4" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="258" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E257" s="4"/>
+    </row>
+    <row r="258" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A258" s="4"/>
       <c r="B258" s="4">
         <v>137507</v>
@@ -3930,8 +4165,9 @@
       <c r="C258" s="4" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="259" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E258" s="4"/>
+    </row>
+    <row r="259" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A259" s="4"/>
       <c r="B259" s="4">
         <v>137509</v>
@@ -3939,8 +4175,9 @@
       <c r="C259" s="4" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="260" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E259" s="4"/>
+    </row>
+    <row r="260" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A260" s="4"/>
       <c r="B260" s="4">
         <v>516903</v>
@@ -3952,15 +4189,16 @@
         <v>149.47</v>
       </c>
     </row>
-    <row r="261" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A261" s="4" t="s">
         <v>282</v>
       </c>
       <c r="B261" s="5"/>
       <c r="C261" s="5"/>
       <c r="D261" s="1"/>
-    </row>
-    <row r="262" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E261" s="5"/>
+    </row>
+    <row r="262" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A262" s="4"/>
       <c r="B262" s="2" t="s">
         <v>204</v>
@@ -3968,8 +4206,9 @@
       <c r="C262" s="4" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="263" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E262" s="4"/>
+    </row>
+    <row r="263" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A263" s="4"/>
       <c r="B263" s="4" t="s">
         <v>138</v>
@@ -3977,8 +4216,9 @@
       <c r="C263" s="4" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="264" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E263" s="4"/>
+    </row>
+    <row r="264" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A264" s="4"/>
       <c r="B264" s="4">
         <v>516972</v>
@@ -3990,7 +4230,7 @@
         <v>26.84</v>
       </c>
     </row>
-    <row r="265" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A265" s="4"/>
       <c r="B265" s="4">
         <v>516971</v>
@@ -4002,13 +4242,13 @@
         <v>24.72</v>
       </c>
     </row>
-    <row r="266" spans="1:4" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="267" spans="1:4" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="268" spans="1:4" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="269" spans="1:4" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="270" spans="1:4" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="271" spans="1:4" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="272" spans="1:4" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="266" spans="1:5" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="267" spans="1:5" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="268" spans="1:5" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="269" spans="1:5" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="270" spans="1:5" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="271" spans="1:5" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="272" spans="1:5" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="273" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="274" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="275" hidden="1" x14ac:dyDescent="0.25"/>
@@ -4051,7 +4291,7 @@
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <protectedRanges>
     <protectedRange sqref="D2:D265" name="Prijs"/>
-    <protectedRange sqref="C2:C265" name="Omschrijving"/>
+    <protectedRange sqref="C2:C265 E2:E265" name="Omschrijving"/>
     <protectedRange sqref="B2:B265" name="Nummer"/>
     <protectedRange sqref="A2:A265" name="Benamingen"/>
   </protectedRanges>

</xml_diff>